<commit_message>
EDIT - possible signals
</commit_message>
<xml_diff>
--- a/data/lista de señales que pueden servir.xlsx
+++ b/data/lista de señales que pueden servir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dacp1\Documents\IAThesis\Brain-Structures-Classification-from-iEEG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A8C970-5B8B-4BE5-8B79-A0D883C6EF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D18D638-0F31-4FDF-A6F7-65637F3DE564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Señales</t>
   </si>
@@ -109,13 +109,34 @@
   </si>
   <si>
     <t>Sí pero es de un milivoltio</t>
+  </si>
+  <si>
+    <t>Parece tener periodicidad/solo está bien la corteza</t>
+  </si>
+  <si>
+    <t>11361009.abf</t>
+  </si>
+  <si>
+    <t>Tálamo POM</t>
+  </si>
+  <si>
+    <t>11361091.abf</t>
+  </si>
+  <si>
+    <t>Tálamo VTM</t>
+  </si>
+  <si>
+    <t>16615005.abf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vM1', 'CA' </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -126,19 +147,34 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBE33D"/>
-        <bgColor rgb="FFFFCC00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -148,8 +184,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFA6"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -162,25 +207,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C16" activeCellId="1" sqref="C20 C16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -608,35 +663,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -650,33 +705,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -690,49 +745,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -746,7 +801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -760,7 +815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -772,6 +827,31 @@
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>